<commit_message>
Se agregaron los ids de periodos a las habitaciones correspondientes. Se comienzan a omitir muchas leyendas que se creaban como "habitacion" (faltan redondear cuestiones como los adicionales, los cuales tienen precio, y por ello mismo no son omitidos por el algoritmo). Tambien las habitaciones pueden contener como precio_string cierta leyenda perteneciente a las aceptadas (sin precio, pero con cierto tipo de "clausura")
</commit_message>
<xml_diff>
--- a/Data/Extracto.xlsx
+++ b/Data/Extracto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oper4\Desktop\Martin\ZGeneral\Nueva carpeta - copia (15)\Nueva carpeta - copia (14)\Nueva carpeta - copia (8)\Mai10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Gerssss\IA\Hoteles\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F4D1B9-A36B-4FD3-892F-ED3EB5E2CDA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5A3626-0FD3-437B-A79F-3DEAD50F0CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10500" xr2:uid="{1224B4C5-8DAE-4381-A3E8-5D9004A18356}"/>
+    <workbookView xWindow="3220" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{1224B4C5-8DAE-4381-A3E8-5D9004A18356}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,18 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -183,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
   <si>
     <r>
       <t xml:space="preserve">Alvear Palace </t>
@@ -1298,6 +1310,15 @@
       </rPr>
       <t xml:space="preserve"> (A)</t>
     </r>
+  </si>
+  <si>
+    <t>Habitacion de Prueba|</t>
+  </si>
+  <si>
+    <t>closing</t>
+  </si>
+  <si>
+    <t>Habitacion de Prueba2</t>
   </si>
 </sst>
 </file>
@@ -1815,7 +1836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2001,6 +2022,19 @@
     <xf numFmtId="0" fontId="33" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2010,18 +2044,8 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2054,7 +2078,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
+      <xdr:rowOff>112395</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2128,7 +2152,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>281940</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>92075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2493,17 +2517,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94E3EAF-DC7A-49A7-8B54-64A4EE873B20}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="133.5546875" customWidth="1"/>
-    <col min="2" max="2" width="58.109375" customWidth="1"/>
+    <col min="1" max="1" width="133.5703125" customWidth="1"/>
+    <col min="2" max="2" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2511,12 +2535,12 @@
       <c r="C1" s="9"/>
       <c r="D1" s="10"/>
       <c r="E1" s="11"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-    </row>
-    <row r="2" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+    </row>
+    <row r="2" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2526,12 +2550,12 @@
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-    </row>
-    <row r="3" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+    </row>
+    <row r="3" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
@@ -2539,12 +2563,12 @@
       <c r="C3" s="19"/>
       <c r="D3" s="20"/>
       <c r="E3" s="21"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-    </row>
-    <row r="4" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+    </row>
+    <row r="4" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A4" s="22"/>
       <c r="B4" s="23" t="s">
         <v>4</v>
@@ -2552,12 +2576,12 @@
       <c r="C4" s="19"/>
       <c r="D4" s="20"/>
       <c r="E4" s="21"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-    </row>
-    <row r="5" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+    </row>
+    <row r="5" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>5</v>
       </c>
@@ -2567,12 +2591,12 @@
       <c r="C5" s="19"/>
       <c r="D5" s="20"/>
       <c r="E5" s="21"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-    </row>
-    <row r="6" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+    </row>
+    <row r="6" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>7</v>
       </c>
@@ -2582,12 +2606,12 @@
       <c r="C6" s="19"/>
       <c r="D6" s="20"/>
       <c r="E6" s="21"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-    </row>
-    <row r="7" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+    </row>
+    <row r="7" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
@@ -2603,12 +2627,12 @@
       <c r="E7" s="27">
         <v>349</v>
       </c>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="78"/>
-    </row>
-    <row r="8" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="75"/>
+    </row>
+    <row r="8" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>9</v>
       </c>
@@ -2624,12 +2648,12 @@
       <c r="E8" s="27">
         <v>433</v>
       </c>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="78"/>
-    </row>
-    <row r="9" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="75"/>
+    </row>
+    <row r="9" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>12</v>
       </c>
@@ -2643,12 +2667,12 @@
       <c r="E9" s="27">
         <v>523</v>
       </c>
-      <c r="G9" s="79"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="78"/>
-    </row>
-    <row r="10" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="75"/>
+    </row>
+    <row r="10" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>13</v>
       </c>
@@ -2662,12 +2686,12 @@
       <c r="E10" s="27">
         <v>591</v>
       </c>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="78"/>
-    </row>
-    <row r="11" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="75"/>
+    </row>
+    <row r="11" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>14</v>
       </c>
@@ -2681,12 +2705,12 @@
       <c r="E11" s="27">
         <v>703</v>
       </c>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="78"/>
-    </row>
-    <row r="12" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="75"/>
+    </row>
+    <row r="12" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>15</v>
       </c>
@@ -2700,23 +2724,23 @@
       <c r="E12" s="27">
         <v>771</v>
       </c>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="78"/>
-    </row>
-    <row r="13" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="75"/>
+    </row>
+    <row r="13" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="27"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="78"/>
-    </row>
-    <row r="14" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="75"/>
+    </row>
+    <row r="14" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>16</v>
       </c>
@@ -2724,12 +2748,12 @@
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="27"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="78"/>
-    </row>
-    <row r="15" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="75"/>
+    </row>
+    <row r="15" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>17</v>
       </c>
@@ -2743,12 +2767,12 @@
       <c r="E15" s="27">
         <v>1125</v>
       </c>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="78"/>
-    </row>
-    <row r="16" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="75"/>
+    </row>
+    <row r="16" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>18</v>
       </c>
@@ -2762,23 +2786,23 @@
       <c r="E16" s="27">
         <v>1215</v>
       </c>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="78"/>
-    </row>
-    <row r="17" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="75"/>
+    </row>
+    <row r="17" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A17" s="24"/>
       <c r="B17" s="25"/>
       <c r="C17" s="19"/>
       <c r="D17" s="20"/>
       <c r="E17" s="27"/>
-      <c r="G17" s="79"/>
-      <c r="H17" s="79"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="78"/>
-    </row>
-    <row r="18" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="75"/>
+    </row>
+    <row r="18" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>19</v>
       </c>
@@ -2786,12 +2810,12 @@
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
       <c r="E18" s="27"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="78"/>
-    </row>
-    <row r="19" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="75"/>
+    </row>
+    <row r="19" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
         <v>20</v>
       </c>
@@ -2805,12 +2829,12 @@
       <c r="E19" s="27">
         <v>1260</v>
       </c>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="80"/>
-      <c r="J19" s="78"/>
-    </row>
-    <row r="20" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="75"/>
+    </row>
+    <row r="20" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>21</v>
       </c>
@@ -2824,12 +2848,12 @@
       <c r="E20" s="27">
         <v>1328</v>
       </c>
-      <c r="G20" s="79"/>
-      <c r="H20" s="79"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="78"/>
-    </row>
-    <row r="21" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="75"/>
+    </row>
+    <row r="21" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>22</v>
       </c>
@@ -2843,12 +2867,12 @@
       <c r="E21" s="27">
         <v>1440</v>
       </c>
-      <c r="G21" s="79"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="78"/>
-    </row>
-    <row r="22" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="75"/>
+    </row>
+    <row r="22" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>23</v>
       </c>
@@ -2862,12 +2886,12 @@
       <c r="E22" s="27">
         <v>1800</v>
       </c>
-      <c r="G22" s="79"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="78"/>
-    </row>
-    <row r="23" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G22" s="76"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="75"/>
+    </row>
+    <row r="23" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>24</v>
       </c>
@@ -2881,24 +2905,24 @@
       <c r="E23" s="27">
         <v>1868</v>
       </c>
-      <c r="G23" s="79"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="78"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-    </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78"/>
-      <c r="J25" s="78"/>
-    </row>
-    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="75"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
+    </row>
+    <row r="26" spans="1:10" ht="21.75" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
         <v>25</v>
       </c>
@@ -2906,12 +2930,12 @@
       <c r="C26" s="33"/>
       <c r="D26" s="34"/>
       <c r="E26" s="35"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-      <c r="J26" s="78"/>
-    </row>
-    <row r="27" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="75"/>
+    </row>
+    <row r="27" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -2921,12 +2945,12 @@
       <c r="C27" s="37"/>
       <c r="D27" s="3"/>
       <c r="E27" s="38"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78"/>
-      <c r="J27" s="78"/>
-    </row>
-    <row r="28" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+    </row>
+    <row r="28" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A28" s="39" t="s">
         <v>26</v>
       </c>
@@ -2936,12 +2960,12 @@
       <c r="C28" s="41"/>
       <c r="D28" s="4"/>
       <c r="E28" s="6"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78"/>
-      <c r="J28" s="78"/>
-    </row>
-    <row r="29" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
+      <c r="J28" s="75"/>
+    </row>
+    <row r="29" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A29" s="42" t="s">
         <v>28</v>
       </c>
@@ -2955,12 +2979,12 @@
       <c r="E29" s="6">
         <v>516</v>
       </c>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="82"/>
-      <c r="J29" s="78"/>
-    </row>
-    <row r="30" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="75"/>
+    </row>
+    <row r="30" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A30" s="42" t="s">
         <v>29</v>
       </c>
@@ -2974,12 +2998,12 @@
       <c r="E30" s="6">
         <v>552</v>
       </c>
-      <c r="G30" s="81"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="82"/>
-      <c r="J30" s="78"/>
-    </row>
-    <row r="31" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="75"/>
+    </row>
+    <row r="31" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A31" s="42" t="s">
         <v>30</v>
       </c>
@@ -2993,12 +3017,12 @@
       <c r="E31" s="6">
         <v>564</v>
       </c>
-      <c r="G31" s="81"/>
-      <c r="H31" s="81"/>
-      <c r="I31" s="82"/>
-      <c r="J31" s="78"/>
-    </row>
-    <row r="32" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G31" s="78"/>
+      <c r="H31" s="78"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="75"/>
+    </row>
+    <row r="32" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A32" s="42" t="s">
         <v>31</v>
       </c>
@@ -3012,12 +3036,12 @@
       <c r="E32" s="6">
         <v>684</v>
       </c>
-      <c r="G32" s="81"/>
-      <c r="H32" s="81"/>
-      <c r="I32" s="82"/>
-      <c r="J32" s="78"/>
-    </row>
-    <row r="33" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G32" s="78"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="79"/>
+      <c r="J32" s="75"/>
+    </row>
+    <row r="33" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A33" s="42" t="s">
         <v>32</v>
       </c>
@@ -3031,12 +3055,12 @@
       <c r="E33" s="6">
         <v>732</v>
       </c>
-      <c r="G33" s="81"/>
-      <c r="H33" s="81"/>
-      <c r="I33" s="82"/>
-      <c r="J33" s="78"/>
-    </row>
-    <row r="34" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G33" s="78"/>
+      <c r="H33" s="78"/>
+      <c r="I33" s="79"/>
+      <c r="J33" s="75"/>
+    </row>
+    <row r="34" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A34" s="42" t="s">
         <v>33</v>
       </c>
@@ -3050,12 +3074,12 @@
       <c r="E34" s="6">
         <v>846</v>
       </c>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="82"/>
-      <c r="J34" s="78"/>
-    </row>
-    <row r="35" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="79"/>
+      <c r="J34" s="75"/>
+    </row>
+    <row r="35" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A35" s="42" t="s">
         <v>34</v>
       </c>
@@ -3069,23 +3093,23 @@
       <c r="E35" s="6">
         <v>924</v>
       </c>
-      <c r="G35" s="81"/>
-      <c r="H35" s="81"/>
-      <c r="I35" s="82"/>
-      <c r="J35" s="78"/>
-    </row>
-    <row r="36" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G35" s="78"/>
+      <c r="H35" s="78"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="75"/>
+    </row>
+    <row r="36" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A36" s="42"/>
       <c r="B36" s="43"/>
       <c r="C36" s="41"/>
       <c r="D36" s="4"/>
       <c r="E36" s="6"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="78"/>
-    </row>
-    <row r="37" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="75"/>
+    </row>
+    <row r="37" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A37" s="44" t="s">
         <v>35</v>
       </c>
@@ -3093,12 +3117,12 @@
       <c r="C37" s="41"/>
       <c r="D37" s="4"/>
       <c r="E37" s="6"/>
-      <c r="G37" s="81"/>
-      <c r="H37" s="81"/>
-      <c r="I37" s="82"/>
-      <c r="J37" s="78"/>
-    </row>
-    <row r="38" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G37" s="78"/>
+      <c r="H37" s="78"/>
+      <c r="I37" s="79"/>
+      <c r="J37" s="75"/>
+    </row>
+    <row r="38" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A38" s="45" t="s">
         <v>36</v>
       </c>
@@ -3106,23 +3130,23 @@
       <c r="C38" s="41"/>
       <c r="D38" s="4"/>
       <c r="E38" s="6"/>
-      <c r="G38" s="81"/>
-      <c r="H38" s="81"/>
-      <c r="I38" s="82"/>
-      <c r="J38" s="78"/>
-    </row>
-    <row r="39" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G38" s="78"/>
+      <c r="H38" s="78"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="75"/>
+    </row>
+    <row r="39" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A39" s="46"/>
       <c r="B39" s="43"/>
       <c r="C39" s="41"/>
       <c r="D39" s="4"/>
       <c r="E39" s="6"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="82"/>
-      <c r="J39" s="78"/>
-    </row>
-    <row r="40" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G39" s="78"/>
+      <c r="H39" s="78"/>
+      <c r="I39" s="79"/>
+      <c r="J39" s="75"/>
+    </row>
+    <row r="40" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A40" s="47" t="s">
         <v>37</v>
       </c>
@@ -3130,23 +3154,23 @@
       <c r="C40" s="41"/>
       <c r="D40" s="4"/>
       <c r="E40" s="6"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="82"/>
-      <c r="J40" s="78"/>
-    </row>
-    <row r="41" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G40" s="78"/>
+      <c r="H40" s="78"/>
+      <c r="I40" s="79"/>
+      <c r="J40" s="75"/>
+    </row>
+    <row r="41" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A41" s="47"/>
       <c r="B41" s="43"/>
       <c r="C41" s="41"/>
       <c r="D41" s="4"/>
       <c r="E41" s="6"/>
-      <c r="G41" s="81"/>
-      <c r="H41" s="81"/>
-      <c r="I41" s="82"/>
-      <c r="J41" s="78"/>
-    </row>
-    <row r="42" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G41" s="78"/>
+      <c r="H41" s="78"/>
+      <c r="I41" s="79"/>
+      <c r="J41" s="75"/>
+    </row>
+    <row r="42" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
         <v>38</v>
       </c>
@@ -3154,12 +3178,12 @@
       <c r="C42" s="41"/>
       <c r="D42" s="4"/>
       <c r="E42" s="6"/>
-      <c r="G42" s="81"/>
-      <c r="H42" s="81"/>
-      <c r="I42" s="82"/>
-      <c r="J42" s="78"/>
-    </row>
-    <row r="43" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G42" s="78"/>
+      <c r="H42" s="78"/>
+      <c r="I42" s="79"/>
+      <c r="J42" s="75"/>
+    </row>
+    <row r="43" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A43" s="42" t="s">
         <v>39</v>
       </c>
@@ -3173,12 +3197,12 @@
       <c r="E43" s="6">
         <v>708</v>
       </c>
-      <c r="G43" s="81"/>
-      <c r="H43" s="81"/>
-      <c r="I43" s="82"/>
-      <c r="J43" s="78"/>
-    </row>
-    <row r="44" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G43" s="78"/>
+      <c r="H43" s="78"/>
+      <c r="I43" s="79"/>
+      <c r="J43" s="75"/>
+    </row>
+    <row r="44" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A44" s="42" t="s">
         <v>40</v>
       </c>
@@ -3192,12 +3216,12 @@
       <c r="E44" s="6">
         <v>816</v>
       </c>
-      <c r="G44" s="81"/>
-      <c r="H44" s="81"/>
-      <c r="I44" s="82"/>
-      <c r="J44" s="78"/>
-    </row>
-    <row r="45" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G44" s="78"/>
+      <c r="H44" s="78"/>
+      <c r="I44" s="79"/>
+      <c r="J44" s="75"/>
+    </row>
+    <row r="45" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A45" s="42" t="s">
         <v>41</v>
       </c>
@@ -3211,12 +3235,12 @@
       <c r="E45" s="6">
         <v>900</v>
       </c>
-      <c r="G45" s="81"/>
-      <c r="H45" s="81"/>
-      <c r="I45" s="82"/>
-      <c r="J45" s="78"/>
-    </row>
-    <row r="46" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G45" s="78"/>
+      <c r="H45" s="78"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="75"/>
+    </row>
+    <row r="46" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A46" s="42" t="s">
         <v>42</v>
       </c>
@@ -3230,23 +3254,23 @@
       <c r="E46" s="6">
         <v>1716</v>
       </c>
-      <c r="G46" s="81"/>
-      <c r="H46" s="81"/>
-      <c r="I46" s="82"/>
-      <c r="J46" s="78"/>
-    </row>
-    <row r="47" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G46" s="78"/>
+      <c r="H46" s="78"/>
+      <c r="I46" s="79"/>
+      <c r="J46" s="75"/>
+    </row>
+    <row r="47" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A47" s="42"/>
       <c r="B47" s="43"/>
       <c r="C47" s="41"/>
       <c r="D47" s="4"/>
       <c r="E47" s="6"/>
-      <c r="G47" s="81"/>
-      <c r="H47" s="81"/>
-      <c r="I47" s="82"/>
-      <c r="J47" s="78"/>
-    </row>
-    <row r="48" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G47" s="78"/>
+      <c r="H47" s="78"/>
+      <c r="I47" s="79"/>
+      <c r="J47" s="75"/>
+    </row>
+    <row r="48" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A48" s="42" t="s">
         <v>43</v>
       </c>
@@ -3254,12 +3278,12 @@
       <c r="C48" s="41"/>
       <c r="D48" s="4"/>
       <c r="E48" s="6"/>
-      <c r="G48" s="81"/>
-      <c r="H48" s="81"/>
-      <c r="I48" s="82"/>
-      <c r="J48" s="78"/>
-    </row>
-    <row r="49" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="79"/>
+      <c r="J48" s="75"/>
+    </row>
+    <row r="49" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A49" s="42" t="s">
         <v>44</v>
       </c>
@@ -3267,23 +3291,23 @@
       <c r="C49" s="41"/>
       <c r="D49" s="4"/>
       <c r="E49" s="6"/>
-      <c r="G49" s="78"/>
-      <c r="H49" s="78"/>
-      <c r="I49" s="78"/>
-      <c r="J49" s="78"/>
-    </row>
-    <row r="50" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G49" s="75"/>
+      <c r="H49" s="75"/>
+      <c r="I49" s="75"/>
+      <c r="J49" s="75"/>
+    </row>
+    <row r="50" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A50" s="48"/>
       <c r="B50" s="43"/>
       <c r="C50" s="41"/>
       <c r="D50" s="4"/>
       <c r="E50" s="6"/>
-      <c r="G50" s="78"/>
-      <c r="H50" s="78"/>
-      <c r="I50" s="78"/>
-      <c r="J50" s="78"/>
-    </row>
-    <row r="51" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G50" s="75"/>
+      <c r="H50" s="75"/>
+      <c r="I50" s="75"/>
+      <c r="J50" s="75"/>
+    </row>
+    <row r="51" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A51" s="47" t="s">
         <v>37</v>
       </c>
@@ -3291,24 +3315,24 @@
       <c r="C51" s="41"/>
       <c r="D51" s="4"/>
       <c r="E51" s="6"/>
-      <c r="G51" s="78"/>
-      <c r="H51" s="78"/>
-      <c r="I51" s="78"/>
-      <c r="J51" s="78"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G52" s="78"/>
-      <c r="H52" s="78"/>
-      <c r="I52" s="78"/>
-      <c r="J52" s="78"/>
-    </row>
-    <row r="53" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G53" s="78"/>
-      <c r="H53" s="78"/>
-      <c r="I53" s="78"/>
-      <c r="J53" s="78"/>
-    </row>
-    <row r="54" spans="1:10" ht="21.6" x14ac:dyDescent="0.4">
+      <c r="G51" s="75"/>
+      <c r="H51" s="75"/>
+      <c r="I51" s="75"/>
+      <c r="J51" s="75"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G52" s="75"/>
+      <c r="H52" s="75"/>
+      <c r="I52" s="75"/>
+      <c r="J52" s="75"/>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G53" s="75"/>
+      <c r="H53" s="75"/>
+      <c r="I53" s="75"/>
+      <c r="J53" s="75"/>
+    </row>
+    <row r="54" spans="1:10" ht="21.75" x14ac:dyDescent="0.3">
       <c r="A54" s="31" t="s">
         <v>67</v>
       </c>
@@ -3316,12 +3340,12 @@
       <c r="C54" s="72"/>
       <c r="D54" s="73"/>
       <c r="E54" s="74"/>
-      <c r="G54" s="78"/>
-      <c r="H54" s="78"/>
-      <c r="I54" s="78"/>
-      <c r="J54" s="78"/>
-    </row>
-    <row r="55" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G54" s="75"/>
+      <c r="H54" s="75"/>
+      <c r="I54" s="75"/>
+      <c r="J54" s="75"/>
+    </row>
+    <row r="55" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>1</v>
       </c>
@@ -3331,12 +3355,12 @@
       <c r="C55" s="2"/>
       <c r="D55" s="50"/>
       <c r="E55" s="51"/>
-      <c r="G55" s="78"/>
-      <c r="H55" s="78"/>
-      <c r="I55" s="78"/>
-      <c r="J55" s="78"/>
-    </row>
-    <row r="56" spans="1:10" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="G55" s="75"/>
+      <c r="H55" s="75"/>
+      <c r="I55" s="75"/>
+      <c r="J55" s="75"/>
+    </row>
+    <row r="56" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A56" s="52"/>
       <c r="B56" s="53" t="s">
         <v>45</v>
@@ -3344,12 +3368,12 @@
       <c r="C56" s="54"/>
       <c r="D56" s="55"/>
       <c r="E56" s="5"/>
-      <c r="G56" s="78"/>
-      <c r="H56" s="78"/>
-      <c r="I56" s="78"/>
-      <c r="J56" s="78"/>
-    </row>
-    <row r="57" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="G56" s="75"/>
+      <c r="H56" s="75"/>
+      <c r="I56" s="75"/>
+      <c r="J56" s="75"/>
+    </row>
+    <row r="57" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A57" s="56" t="s">
         <v>46</v>
       </c>
@@ -3359,23 +3383,23 @@
       <c r="C57" s="54"/>
       <c r="D57" s="55"/>
       <c r="E57" s="5"/>
-      <c r="G57" s="78"/>
-      <c r="H57" s="78"/>
-      <c r="I57" s="78"/>
-      <c r="J57" s="78"/>
-    </row>
-    <row r="58" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="G57" s="75"/>
+      <c r="H57" s="75"/>
+      <c r="I57" s="75"/>
+      <c r="J57" s="75"/>
+    </row>
+    <row r="58" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A58" s="52"/>
       <c r="B58" s="58"/>
       <c r="C58" s="54"/>
       <c r="D58" s="55"/>
       <c r="E58" s="5"/>
-      <c r="G58" s="78"/>
-      <c r="H58" s="78"/>
-      <c r="I58" s="78"/>
-      <c r="J58" s="78"/>
-    </row>
-    <row r="59" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G58" s="75"/>
+      <c r="H58" s="75"/>
+      <c r="I58" s="75"/>
+      <c r="J58" s="75"/>
+    </row>
+    <row r="59" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A59" s="59" t="s">
         <v>48</v>
       </c>
@@ -3383,12 +3407,12 @@
       <c r="C59" s="61"/>
       <c r="D59" s="3"/>
       <c r="E59" s="62"/>
-      <c r="G59" s="78"/>
-      <c r="H59" s="78"/>
-      <c r="I59" s="78"/>
-      <c r="J59" s="78"/>
-    </row>
-    <row r="60" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G59" s="75"/>
+      <c r="H59" s="75"/>
+      <c r="I59" s="75"/>
+      <c r="J59" s="75"/>
+    </row>
+    <row r="60" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A60" s="63" t="s">
         <v>49</v>
       </c>
@@ -3404,12 +3428,12 @@
       <c r="E60" s="6">
         <v>261</v>
       </c>
-      <c r="G60" s="81"/>
-      <c r="H60" s="81"/>
-      <c r="I60" s="82"/>
-      <c r="J60" s="78"/>
-    </row>
-    <row r="61" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G60" s="78"/>
+      <c r="H60" s="78"/>
+      <c r="I60" s="79"/>
+      <c r="J60" s="75"/>
+    </row>
+    <row r="61" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A61" s="63" t="s">
         <v>51</v>
       </c>
@@ -3425,12 +3449,12 @@
       <c r="E61" s="6">
         <v>324</v>
       </c>
-      <c r="G61" s="81"/>
-      <c r="H61" s="81"/>
-      <c r="I61" s="82"/>
-      <c r="J61" s="78"/>
-    </row>
-    <row r="62" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G61" s="78"/>
+      <c r="H61" s="78"/>
+      <c r="I61" s="79"/>
+      <c r="J61" s="75"/>
+    </row>
+    <row r="62" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A62" s="63" t="s">
         <v>53</v>
       </c>
@@ -3446,12 +3470,12 @@
       <c r="E62" s="6">
         <v>342</v>
       </c>
-      <c r="G62" s="81"/>
-      <c r="H62" s="81"/>
-      <c r="I62" s="82"/>
-      <c r="J62" s="78"/>
-    </row>
-    <row r="63" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G62" s="78"/>
+      <c r="H62" s="78"/>
+      <c r="I62" s="79"/>
+      <c r="J62" s="75"/>
+    </row>
+    <row r="63" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A63" s="63" t="s">
         <v>55</v>
       </c>
@@ -3467,12 +3491,12 @@
       <c r="E63" s="6">
         <v>459</v>
       </c>
-      <c r="G63" s="81"/>
-      <c r="H63" s="81"/>
-      <c r="I63" s="82"/>
-      <c r="J63" s="78"/>
-    </row>
-    <row r="64" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G63" s="78"/>
+      <c r="H63" s="78"/>
+      <c r="I63" s="79"/>
+      <c r="J63" s="75"/>
+    </row>
+    <row r="64" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A64" s="67" t="s">
         <v>56</v>
       </c>
@@ -3486,12 +3510,12 @@
       <c r="E64" s="6">
         <v>459</v>
       </c>
-      <c r="G64" s="81"/>
-      <c r="H64" s="81"/>
-      <c r="I64" s="82"/>
-      <c r="J64" s="78"/>
-    </row>
-    <row r="65" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G64" s="78"/>
+      <c r="H64" s="78"/>
+      <c r="I64" s="79"/>
+      <c r="J64" s="75"/>
+    </row>
+    <row r="65" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A65" s="63" t="s">
         <v>57</v>
       </c>
@@ -3505,12 +3529,12 @@
       <c r="E65" s="6">
         <v>563</v>
       </c>
-      <c r="G65" s="81"/>
-      <c r="H65" s="81"/>
-      <c r="I65" s="82"/>
-      <c r="J65" s="78"/>
-    </row>
-    <row r="66" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G65" s="78"/>
+      <c r="H65" s="78"/>
+      <c r="I65" s="79"/>
+      <c r="J65" s="75"/>
+    </row>
+    <row r="66" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A66" s="63" t="s">
         <v>58</v>
       </c>
@@ -3524,12 +3548,12 @@
       <c r="E66" s="6">
         <v>783</v>
       </c>
-      <c r="G66" s="81"/>
-      <c r="H66" s="81"/>
-      <c r="I66" s="82"/>
-      <c r="J66" s="78"/>
-    </row>
-    <row r="67" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G66" s="78"/>
+      <c r="H66" s="78"/>
+      <c r="I66" s="79"/>
+      <c r="J66" s="75"/>
+    </row>
+    <row r="67" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A67" s="63" t="s">
         <v>59</v>
       </c>
@@ -3543,12 +3567,12 @@
       <c r="E67" s="6">
         <v>2070</v>
       </c>
-      <c r="G67" s="81"/>
-      <c r="H67" s="81"/>
-      <c r="I67" s="82"/>
-      <c r="J67" s="78"/>
-    </row>
-    <row r="68" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G67" s="78"/>
+      <c r="H67" s="78"/>
+      <c r="I67" s="79"/>
+      <c r="J67" s="75"/>
+    </row>
+    <row r="68" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A68" s="68" t="s">
         <v>60</v>
       </c>
@@ -3562,12 +3586,12 @@
       <c r="E68" s="6">
         <v>1035</v>
       </c>
-      <c r="G68" s="81"/>
-      <c r="H68" s="81"/>
-      <c r="I68" s="82"/>
-      <c r="J68" s="78"/>
-    </row>
-    <row r="69" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G68" s="78"/>
+      <c r="H68" s="78"/>
+      <c r="I68" s="79"/>
+      <c r="J68" s="75"/>
+    </row>
+    <row r="69" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A69" s="63" t="s">
         <v>61</v>
       </c>
@@ -3581,12 +3605,12 @@
       <c r="E69" s="6">
         <v>738</v>
       </c>
-      <c r="G69" s="81"/>
-      <c r="H69" s="81"/>
-      <c r="I69" s="82"/>
-      <c r="J69" s="78"/>
-    </row>
-    <row r="70" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G69" s="78"/>
+      <c r="H69" s="78"/>
+      <c r="I69" s="79"/>
+      <c r="J69" s="75"/>
+    </row>
+    <row r="70" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A70" s="63" t="s">
         <v>62</v>
       </c>
@@ -3600,12 +3624,12 @@
       <c r="E70" s="6">
         <v>945</v>
       </c>
-      <c r="G70" s="81"/>
-      <c r="H70" s="81"/>
-      <c r="I70" s="82"/>
-      <c r="J70" s="78"/>
-    </row>
-    <row r="71" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G70" s="78"/>
+      <c r="H70" s="78"/>
+      <c r="I70" s="79"/>
+      <c r="J70" s="75"/>
+    </row>
+    <row r="71" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A71" s="63" t="s">
         <v>63</v>
       </c>
@@ -3619,12 +3643,12 @@
       <c r="E71" s="6">
         <v>1800</v>
       </c>
-      <c r="G71" s="81"/>
-      <c r="H71" s="81"/>
-      <c r="I71" s="82"/>
-      <c r="J71" s="78"/>
-    </row>
-    <row r="72" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G71" s="78"/>
+      <c r="H71" s="78"/>
+      <c r="I71" s="79"/>
+      <c r="J71" s="75"/>
+    </row>
+    <row r="72" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A72" s="63" t="s">
         <v>64</v>
       </c>
@@ -3638,148 +3662,148 @@
       <c r="E72" s="6">
         <v>2520</v>
       </c>
-      <c r="G72" s="81"/>
-      <c r="H72" s="81"/>
-      <c r="I72" s="82"/>
-      <c r="J72" s="78"/>
-    </row>
-    <row r="73" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="G72" s="78"/>
+      <c r="H72" s="78"/>
+      <c r="I72" s="79"/>
+      <c r="J72" s="75"/>
+    </row>
+    <row r="73" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A73" s="69"/>
       <c r="B73" s="65"/>
       <c r="C73" s="54"/>
       <c r="D73" s="4"/>
       <c r="E73" s="70"/>
-      <c r="G73" s="81"/>
-      <c r="H73" s="81"/>
-      <c r="I73" s="82"/>
-      <c r="J73" s="78"/>
-    </row>
-    <row r="74" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="G73" s="78"/>
+      <c r="H73" s="78"/>
+      <c r="I73" s="79"/>
+      <c r="J73" s="75"/>
+    </row>
+    <row r="74" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A74" s="63" t="s">
         <v>49</v>
       </c>
       <c r="B74" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="C74" s="75" t="s">
+      <c r="C74" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="D74" s="76"/>
-      <c r="E74" s="77"/>
-      <c r="G74" s="78"/>
-      <c r="H74" s="78"/>
-      <c r="I74" s="78"/>
-      <c r="J74" s="78"/>
-    </row>
-    <row r="75" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="D74" s="81"/>
+      <c r="E74" s="82"/>
+      <c r="G74" s="75"/>
+      <c r="H74" s="75"/>
+      <c r="I74" s="75"/>
+      <c r="J74" s="75"/>
+    </row>
+    <row r="75" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A75" s="63" t="s">
         <v>51</v>
       </c>
       <c r="B75" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="C75" s="75"/>
-      <c r="D75" s="76"/>
-      <c r="E75" s="77"/>
-      <c r="G75" s="78"/>
-      <c r="H75" s="78"/>
-      <c r="I75" s="78"/>
-      <c r="J75" s="78"/>
-    </row>
-    <row r="76" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="C75" s="80"/>
+      <c r="D75" s="81"/>
+      <c r="E75" s="82"/>
+      <c r="G75" s="75"/>
+      <c r="H75" s="75"/>
+      <c r="I75" s="75"/>
+      <c r="J75" s="75"/>
+    </row>
+    <row r="76" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A76" s="63" t="s">
         <v>53</v>
       </c>
       <c r="B76" s="65"/>
-      <c r="C76" s="75"/>
-      <c r="D76" s="76"/>
-      <c r="E76" s="77"/>
-      <c r="G76" s="78"/>
-      <c r="H76" s="78"/>
-      <c r="I76" s="78"/>
-      <c r="J76" s="78"/>
-    </row>
-    <row r="77" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="C76" s="80"/>
+      <c r="D76" s="81"/>
+      <c r="E76" s="82"/>
+      <c r="G76" s="75"/>
+      <c r="H76" s="75"/>
+      <c r="I76" s="75"/>
+      <c r="J76" s="75"/>
+    </row>
+    <row r="77" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A77" s="63" t="s">
         <v>55</v>
       </c>
       <c r="B77" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="C77" s="75"/>
-      <c r="D77" s="76"/>
-      <c r="E77" s="77"/>
-      <c r="G77" s="78"/>
-      <c r="H77" s="78"/>
-      <c r="I77" s="78"/>
-      <c r="J77" s="78"/>
-    </row>
-    <row r="78" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="C77" s="80"/>
+      <c r="D77" s="81"/>
+      <c r="E77" s="82"/>
+      <c r="G77" s="75"/>
+      <c r="H77" s="75"/>
+      <c r="I77" s="75"/>
+      <c r="J77" s="75"/>
+    </row>
+    <row r="78" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A78" s="67" t="s">
         <v>56</v>
       </c>
       <c r="B78" s="65"/>
-      <c r="C78" s="75"/>
-      <c r="D78" s="76"/>
-      <c r="E78" s="77"/>
-      <c r="G78" s="78"/>
-      <c r="H78" s="78"/>
-      <c r="I78" s="78"/>
-      <c r="J78" s="78"/>
-    </row>
-    <row r="79" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="C78" s="80"/>
+      <c r="D78" s="81"/>
+      <c r="E78" s="82"/>
+      <c r="G78" s="75"/>
+      <c r="H78" s="75"/>
+      <c r="I78" s="75"/>
+      <c r="J78" s="75"/>
+    </row>
+    <row r="79" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A79" s="63" t="s">
         <v>57</v>
       </c>
       <c r="B79" s="65"/>
-      <c r="C79" s="75"/>
-      <c r="D79" s="76"/>
-      <c r="E79" s="77"/>
-      <c r="G79" s="78"/>
-      <c r="H79" s="78"/>
-      <c r="I79" s="78"/>
-      <c r="J79" s="78"/>
-    </row>
-    <row r="80" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="C79" s="80"/>
+      <c r="D79" s="81"/>
+      <c r="E79" s="82"/>
+      <c r="G79" s="75"/>
+      <c r="H79" s="75"/>
+      <c r="I79" s="75"/>
+      <c r="J79" s="75"/>
+    </row>
+    <row r="80" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A80" s="63" t="s">
         <v>58</v>
       </c>
       <c r="B80" s="65"/>
-      <c r="C80" s="75"/>
-      <c r="D80" s="76"/>
-      <c r="E80" s="77"/>
-      <c r="G80" s="78"/>
-      <c r="H80" s="78"/>
-      <c r="I80" s="78"/>
-      <c r="J80" s="78"/>
-    </row>
-    <row r="81" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="C80" s="80"/>
+      <c r="D80" s="81"/>
+      <c r="E80" s="82"/>
+      <c r="G80" s="75"/>
+      <c r="H80" s="75"/>
+      <c r="I80" s="75"/>
+      <c r="J80" s="75"/>
+    </row>
+    <row r="81" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A81" s="63" t="s">
         <v>59</v>
       </c>
       <c r="B81" s="65"/>
-      <c r="C81" s="75"/>
-      <c r="D81" s="76"/>
-      <c r="E81" s="77"/>
-      <c r="G81" s="78"/>
-      <c r="H81" s="78"/>
-      <c r="I81" s="78"/>
-      <c r="J81" s="78"/>
-    </row>
-    <row r="82" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="C81" s="80"/>
+      <c r="D81" s="81"/>
+      <c r="E81" s="82"/>
+      <c r="G81" s="75"/>
+      <c r="H81" s="75"/>
+      <c r="I81" s="75"/>
+      <c r="J81" s="75"/>
+    </row>
+    <row r="82" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A82" s="68" t="s">
         <v>60</v>
       </c>
       <c r="B82" s="65"/>
-      <c r="C82" s="75"/>
-      <c r="D82" s="76"/>
-      <c r="E82" s="77"/>
-      <c r="G82" s="78"/>
-      <c r="H82" s="78"/>
-      <c r="I82" s="78"/>
-      <c r="J82" s="78"/>
-    </row>
-    <row r="83" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="C82" s="80"/>
+      <c r="D82" s="81"/>
+      <c r="E82" s="82"/>
+      <c r="G82" s="75"/>
+      <c r="H82" s="75"/>
+      <c r="I82" s="75"/>
+      <c r="J82" s="75"/>
+    </row>
+    <row r="83" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A83" s="63" t="s">
         <v>61</v>
       </c>
@@ -3793,12 +3817,12 @@
       <c r="E83" s="6">
         <v>810</v>
       </c>
-      <c r="G83" s="81"/>
-      <c r="H83" s="81"/>
-      <c r="I83" s="82"/>
-      <c r="J83" s="78"/>
-    </row>
-    <row r="84" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G83" s="78"/>
+      <c r="H83" s="78"/>
+      <c r="I83" s="79"/>
+      <c r="J83" s="75"/>
+    </row>
+    <row r="84" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A84" s="63" t="s">
         <v>62</v>
       </c>
@@ -3812,12 +3836,12 @@
       <c r="E84" s="6">
         <v>1035</v>
       </c>
-      <c r="G84" s="81"/>
-      <c r="H84" s="81"/>
-      <c r="I84" s="82"/>
-      <c r="J84" s="78"/>
-    </row>
-    <row r="85" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G84" s="78"/>
+      <c r="H84" s="78"/>
+      <c r="I84" s="79"/>
+      <c r="J84" s="75"/>
+    </row>
+    <row r="85" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A85" s="63" t="s">
         <v>63</v>
       </c>
@@ -3831,12 +3855,12 @@
       <c r="E85" s="6">
         <v>1980</v>
       </c>
-      <c r="G85" s="81"/>
-      <c r="H85" s="81"/>
-      <c r="I85" s="82"/>
-      <c r="J85" s="78"/>
-    </row>
-    <row r="86" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="G85" s="78"/>
+      <c r="H85" s="78"/>
+      <c r="I85" s="79"/>
+      <c r="J85" s="75"/>
+    </row>
+    <row r="86" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A86" s="63" t="s">
         <v>64</v>
       </c>
@@ -3850,40 +3874,52 @@
       <c r="E86" s="6">
         <v>2790</v>
       </c>
-      <c r="G86" s="81"/>
-      <c r="H86" s="81"/>
-      <c r="I86" s="82"/>
-      <c r="J86" s="78"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G87" s="78"/>
-      <c r="H87" s="78"/>
-      <c r="I87" s="78"/>
-      <c r="J87" s="78"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G88" s="78"/>
-      <c r="H88" s="78"/>
-      <c r="I88" s="78"/>
-      <c r="J88" s="78"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G89" s="78"/>
-      <c r="H89" s="78"/>
-      <c r="I89" s="78"/>
-      <c r="J89" s="78"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G90" s="78"/>
-      <c r="H90" s="78"/>
-      <c r="I90" s="78"/>
-      <c r="J90" s="78"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G91" s="78"/>
-      <c r="H91" s="78"/>
-      <c r="I91" s="78"/>
-      <c r="J91" s="78"/>
+      <c r="G86" s="78"/>
+      <c r="H86" s="78"/>
+      <c r="I86" s="79"/>
+      <c r="J86" s="75"/>
+    </row>
+    <row r="87" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="C87" t="s">
+        <v>69</v>
+      </c>
+      <c r="G87" s="75"/>
+      <c r="H87" s="75"/>
+      <c r="I87" s="75"/>
+      <c r="J87" s="75"/>
+    </row>
+    <row r="88" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="C88" s="76">
+        <v>2500.4499999999998</v>
+      </c>
+      <c r="G88" s="75"/>
+      <c r="H88" s="75"/>
+      <c r="I88" s="75"/>
+      <c r="J88" s="75"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G89" s="75"/>
+      <c r="H89" s="75"/>
+      <c r="I89" s="75"/>
+      <c r="J89" s="75"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G90" s="75"/>
+      <c r="H90" s="75"/>
+      <c r="I90" s="75"/>
+      <c r="J90" s="75"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G91" s="75"/>
+      <c r="H91" s="75"/>
+      <c r="I91" s="75"/>
+      <c r="J91" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>